<commit_message>
Fixed first 3 columns when scrolling horizontally
</commit_message>
<xml_diff>
--- a/Inventory/Inventory.xlsx
+++ b/Inventory/Inventory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanfung/Documents/GitLab/Personal/Inventory-Management-System/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanfung/Documents/GitLab/Personal/Inventory-Management-System/Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3875154-B2F6-F544-8B22-C1386DBC1019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539EC207-2BF1-3F42-BFAE-EC7B6E868496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Barcode</t>
   </si>
@@ -128,16 +128,46 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,12 +213,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB841EA0-60E6-224F-AB38-922C9B8D814D}" name="Library" displayName="Library" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11" xr:uid="{A37492C6-07E7-654F-97DE-0A55DFE07177}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB841EA0-60E6-224F-AB38-922C9B8D814D}" name="Library" displayName="Library" ref="A1:K11" totalsRowShown="0">
+  <autoFilter ref="A1:K11" xr:uid="{A37492C6-07E7-654F-97DE-0A55DFE07177}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F71BDC08-53F1-3542-A90C-6FD75AF4E5F2}" name="Barcode"/>
     <tableColumn id="2" xr3:uid="{A608C74C-1909-2D4D-9548-B6BAB654E1CC}" name="Name"/>
     <tableColumn id="3" xr3:uid="{CA051405-93A1-FB4F-BFFA-3C3F622E7480}" name="Location"/>
+    <tableColumn id="4" xr3:uid="{602BA418-0E31-F84F-91A3-BD33581AAA2C}" name="Column1"/>
+    <tableColumn id="5" xr3:uid="{69D35D59-E04C-9940-BC1E-6177921EAC4D}" name="Column2"/>
+    <tableColumn id="6" xr3:uid="{51FBB895-8C99-C54F-BE52-0497E650F553}" name="Column3"/>
+    <tableColumn id="7" xr3:uid="{C111C4B1-F976-9147-860E-9DC4ED98C213}" name="Column4"/>
+    <tableColumn id="8" xr3:uid="{2B24AE0D-6463-8345-89D9-B7FA7629D8A0}" name="Column5"/>
+    <tableColumn id="9" xr3:uid="{C5528EA1-EC6A-5F4C-AF28-B6BA31D0E38F}" name="Column6"/>
+    <tableColumn id="10" xr3:uid="{F4D2BEB3-2B9F-D148-BCB8-72F4B928657A}" name="Column7"/>
+    <tableColumn id="11" xr3:uid="{E4CBBF5F-8015-9E40-9CB7-EBE2021257C6}" name="Column8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -502,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFF6BC4-A1CC-6C45-B003-D83E9A7F5B9B}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -515,7 +553,7 @@
     <col min="3" max="3" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,8 +563,32 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -534,7 +596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -542,7 +604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -550,7 +612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -558,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -566,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -574,7 +636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -582,7 +644,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -590,7 +652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -598,7 +660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -607,6 +669,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Added fixed headers for vertical scrolling
</commit_message>
<xml_diff>
--- a/Inventory/Inventory.xlsx
+++ b/Inventory/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanfung/Documents/GitLab/Personal/Inventory-Management-System/Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539EC207-2BF1-3F42-BFAE-EC7B6E868496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EC047A-6C6E-D245-AB6B-8DA42041122A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Barcode</t>
   </si>
@@ -213,8 +213,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB841EA0-60E6-224F-AB38-922C9B8D814D}" name="Library" displayName="Library" ref="A1:K11" totalsRowShown="0">
-  <autoFilter ref="A1:K11" xr:uid="{A37492C6-07E7-654F-97DE-0A55DFE07177}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB841EA0-60E6-224F-AB38-922C9B8D814D}" name="Library" displayName="Library" ref="A1:K31" totalsRowShown="0">
+  <autoFilter ref="A1:K31" xr:uid="{A37492C6-07E7-654F-97DE-0A55DFE07177}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F71BDC08-53F1-3542-A90C-6FD75AF4E5F2}" name="Barcode"/>
     <tableColumn id="2" xr3:uid="{A608C74C-1909-2D4D-9548-B6BAB654E1CC}" name="Name"/>
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFF6BC4-A1CC-6C45-B003-D83E9A7F5B9B}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -665,6 +665,166 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created separate tabs for each panel
</commit_message>
<xml_diff>
--- a/Inventory/Inventory.xlsx
+++ b/Inventory/Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/susanfung/Documents/GitLab/Personal/Inventory-Management-System/Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EC047A-6C6E-D245-AB6B-8DA42041122A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0020450C-0441-2941-9E54-0980ABADB019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Barcode</t>
   </si>
@@ -152,6 +152,54 @@
   </si>
   <si>
     <t>Column8</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -213,8 +261,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB841EA0-60E6-224F-AB38-922C9B8D814D}" name="Library" displayName="Library" ref="A1:K31" totalsRowShown="0">
-  <autoFilter ref="A1:K31" xr:uid="{A37492C6-07E7-654F-97DE-0A55DFE07177}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB841EA0-60E6-224F-AB38-922C9B8D814D}" name="Library" displayName="Library" ref="A1:K27" totalsRowShown="0">
+  <autoFilter ref="A1:K27" xr:uid="{A37492C6-07E7-654F-97DE-0A55DFE07177}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F71BDC08-53F1-3542-A90C-6FD75AF4E5F2}" name="Barcode"/>
     <tableColumn id="2" xr3:uid="{A608C74C-1909-2D4D-9548-B6BAB654E1CC}" name="Name"/>
@@ -540,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFF6BC4-A1CC-6C45-B003-D83E9A7F5B9B}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -673,7 +721,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -681,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -689,7 +737,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -697,7 +745,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -705,7 +753,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -713,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -721,7 +769,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -729,7 +777,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -737,7 +785,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -745,7 +793,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -753,7 +801,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -761,7 +809,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -769,7 +817,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -777,7 +825,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -785,7 +833,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -793,39 +841,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>